<commit_message>
Removed Tiger search bug
</commit_message>
<xml_diff>
--- a/data/csv_wtds/evolve.xlsx
+++ b/data/csv_wtds/evolve.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
   <si>
     <t>ae</t>
   </si>
@@ -41,91 +41,94 @@
     <t>asdg</t>
   </si>
   <si>
+    <t>gam id</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>adsfasdf</t>
+  </si>
+  <si>
+    <t>asdfadsf</t>
+  </si>
+  <si>
+    <t>adfdsf</t>
+  </si>
+  <si>
+    <t>adfsdf</t>
+  </si>
+  <si>
+    <t>adsfdf</t>
+  </si>
+  <si>
+    <t>adsfsdf</t>
+  </si>
+  <si>
+    <t>adfaf</t>
+  </si>
+  <si>
+    <t>adff</t>
+  </si>
+  <si>
+    <t>asdff</t>
+  </si>
+  <si>
+    <t>adsfasdfd</t>
+  </si>
+  <si>
+    <t>adsgasdg</t>
+  </si>
+  <si>
+    <t>adsggda</t>
+  </si>
+  <si>
+    <t>dgg</t>
+  </si>
+  <si>
+    <t>asdgga</t>
+  </si>
+  <si>
+    <t>adsgagd</t>
+  </si>
+  <si>
+    <t>asdggdsa</t>
+  </si>
+  <si>
+    <t>adsgadsg</t>
+  </si>
+  <si>
+    <t>adgasdg</t>
+  </si>
+  <si>
+    <t>asdgadsg</t>
+  </si>
+  <si>
+    <t>MRC</t>
+  </si>
+  <si>
+    <t>NRC</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>dsfa</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>adf</t>
+  </si>
+  <si>
     <t>fasdf</t>
-  </si>
-  <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>adsfasdf</t>
-  </si>
-  <si>
-    <t>asdfadsf</t>
-  </si>
-  <si>
-    <t>adfdsf</t>
-  </si>
-  <si>
-    <t>adfsdf</t>
-  </si>
-  <si>
-    <t>adsfdf</t>
-  </si>
-  <si>
-    <t>adsfsdf</t>
-  </si>
-  <si>
-    <t>adfaf</t>
-  </si>
-  <si>
-    <t>adff</t>
-  </si>
-  <si>
-    <t>asdff</t>
-  </si>
-  <si>
-    <t>adsfasdfd</t>
-  </si>
-  <si>
-    <t>adsgasdg</t>
-  </si>
-  <si>
-    <t>adsggda</t>
-  </si>
-  <si>
-    <t>dgg</t>
-  </si>
-  <si>
-    <t>asdgga</t>
-  </si>
-  <si>
-    <t>adsgagd</t>
-  </si>
-  <si>
-    <t>asdggdsa</t>
-  </si>
-  <si>
-    <t>adsgadsg</t>
-  </si>
-  <si>
-    <t>adgasdg</t>
-  </si>
-  <si>
-    <t>asdgadsg</t>
-  </si>
-  <si>
-    <t>MRC</t>
-  </si>
-  <si>
-    <t>NRC</t>
-  </si>
-  <si>
-    <t>adsf</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>dsfa</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>ads</t>
-  </si>
-  <si>
-    <t>adf</t>
   </si>
   <si>
     <t>fasd</t>
@@ -245,8 +248,8 @@
   </sheetPr>
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU4" activeCellId="0" sqref="AU4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -429,13 +432,13 @@
         <v>817964</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>11</v>
@@ -519,7 +522,7 @@
         <v>100</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AP2" s="0" t="s">
         <v>31</v>
@@ -537,12 +540,12 @@
         <v>31</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AL3" s="0" t="n">
         <v>200</v>
@@ -551,13 +554,13 @@
         <v>200</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AP3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AR3" s="0" t="s">
         <v>31</v>
@@ -569,7 +572,7 @@
         <v>31</v>
       </c>
       <c r="AU3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>